<commit_message>
Deploy: Update site content, preserve CNAME, add .nojekyll
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-onc-observation-codes.xlsx
+++ b/docs/CodeSystem-onc-observation-codes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="196">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-26T14:13:58+00:00</t>
+    <t>2025-12-26T15:22:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -108,7 +108,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>30</t>
+    <t>53</t>
   </si>
   <si>
     <t>Level</t>
@@ -394,6 +394,213 @@
   </si>
   <si>
     <t>Deeply pigmented dark brown to black; never burns, tans very easily</t>
+  </si>
+  <si>
+    <t>what-matters</t>
+  </si>
+  <si>
+    <t>What Matters to Me</t>
+  </si>
+  <si>
+    <t>Patient-identified priorities and non-clinical goals</t>
+  </si>
+  <si>
+    <t>patient-story</t>
+  </si>
+  <si>
+    <t>Patient Story</t>
+  </si>
+  <si>
+    <t>Narrative summary of patient background, preferences, and autobiography</t>
+  </si>
+  <si>
+    <t>relational-engagement</t>
+  </si>
+  <si>
+    <t>Relational Engagement Score</t>
+  </si>
+  <si>
+    <t>Assessment of the quality of nurse-patient engagement (1-5)</t>
+  </si>
+  <si>
+    <t>cfs-score</t>
+  </si>
+  <si>
+    <t>Clinical Frailty Scale Score</t>
+  </si>
+  <si>
+    <t>Total score for Rockwood Clinical Frailty Scale</t>
+  </si>
+  <si>
+    <t>cfs-1</t>
+  </si>
+  <si>
+    <t>Very Fit</t>
+  </si>
+  <si>
+    <t>Robus, active, energetic and motivated</t>
+  </si>
+  <si>
+    <t>cfs-2</t>
+  </si>
+  <si>
+    <t>Well</t>
+  </si>
+  <si>
+    <t>No active disease symptoms but less fit than category 1</t>
+  </si>
+  <si>
+    <t>cfs-3</t>
+  </si>
+  <si>
+    <t>Managing Well</t>
+  </si>
+  <si>
+    <t>Medical problems are well controlled, but not regularly active</t>
+  </si>
+  <si>
+    <t>cfs-4</t>
+  </si>
+  <si>
+    <t>Vulnerable</t>
+  </si>
+  <si>
+    <t>Not dependent for daily help, but symptoms limit activities</t>
+  </si>
+  <si>
+    <t>cfs-5</t>
+  </si>
+  <si>
+    <t>Mildly Frail</t>
+  </si>
+  <si>
+    <t>Need help with high order IADLs (finances, transportation, heavy housework)</t>
+  </si>
+  <si>
+    <t>cfs-6</t>
+  </si>
+  <si>
+    <t>Moderately Frail</t>
+  </si>
+  <si>
+    <t>Need help with all outside activities and some housekeeping</t>
+  </si>
+  <si>
+    <t>cfs-7</t>
+  </si>
+  <si>
+    <t>Severely Frail</t>
+  </si>
+  <si>
+    <t>Completely dependent for personal care</t>
+  </si>
+  <si>
+    <t>cfs-8</t>
+  </si>
+  <si>
+    <t>Very Severely Frail</t>
+  </si>
+  <si>
+    <t>Completely dependent, approaching end of life</t>
+  </si>
+  <si>
+    <t>cfs-9</t>
+  </si>
+  <si>
+    <t>Terminally Ill</t>
+  </si>
+  <si>
+    <t>Approaching the end of life (life expectancy &lt;6 months)</t>
+  </si>
+  <si>
+    <t>4at-score</t>
+  </si>
+  <si>
+    <t>4AT Delirium Score</t>
+  </si>
+  <si>
+    <t>Total score for 4AT assessment</t>
+  </si>
+  <si>
+    <t>4at-alertness</t>
+  </si>
+  <si>
+    <t>Alertness</t>
+  </si>
+  <si>
+    <t>4AT Item 1: Alertness</t>
+  </si>
+  <si>
+    <t>4at-amt4</t>
+  </si>
+  <si>
+    <t>AMT4 Score</t>
+  </si>
+  <si>
+    <t>4AT Item 2: Abbreviated Mental Test 4</t>
+  </si>
+  <si>
+    <t>4at-attention</t>
+  </si>
+  <si>
+    <t>Attention</t>
+  </si>
+  <si>
+    <t>4AT Item 3: Attention (Months Backwards)</t>
+  </si>
+  <si>
+    <t>4at-acute-change</t>
+  </si>
+  <si>
+    <t>Acute Change</t>
+  </si>
+  <si>
+    <t>4AT Item 4: Acute Change or Fluctuating Course</t>
+  </si>
+  <si>
+    <t>reasonable-adjustment</t>
+  </si>
+  <si>
+    <t>Reasonable Adjustment</t>
+  </si>
+  <si>
+    <t>Requirement for adjustment to care delivery (Equality Act)</t>
+  </si>
+  <si>
+    <t>mca-assessment</t>
+  </si>
+  <si>
+    <t>Mental Capacity Assessment</t>
+  </si>
+  <si>
+    <t>Assessment of capacity to make a specific decision</t>
+  </si>
+  <si>
+    <t>capacity-present</t>
+  </si>
+  <si>
+    <t>Capacity Present</t>
+  </si>
+  <si>
+    <t>Patient has capacity for this decision</t>
+  </si>
+  <si>
+    <t>capacity-absent</t>
+  </si>
+  <si>
+    <t>Capacity Absent</t>
+  </si>
+  <si>
+    <t>Patient lacks capacity for this decision</t>
+  </si>
+  <si>
+    <t>best-interest</t>
+  </si>
+  <si>
+    <t>Best Interest Decision</t>
+  </si>
+  <si>
+    <t>Decision made in patient's best interest</t>
   </si>
 </sst>
 </file>
@@ -692,7 +899,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1132,6 +1339,328 @@
         <v>126</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="D32" t="s" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="D33" t="s" s="2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="D34" t="s" s="2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="D35" t="s" s="2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="D36" t="s" s="2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="D37" t="s" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="D38" t="s" s="2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="D39" t="s" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="D40" t="s" s="2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="C41" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="D41" t="s" s="2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="D42" t="s" s="2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="D43" t="s" s="2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="C44" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="D44" t="s" s="2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="D45" t="s" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s" s="2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="D47" t="s" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="D48" t="s" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="D49" t="s" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="D50" t="s" s="2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="D51" t="s" s="2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="D52" t="s" s="2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="D53" t="s" s="2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="D54" t="s" s="2">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>